<commit_message>
updates for Arctos transform
</commit_message>
<xml_diff>
--- a/input/Lewis World Species List 26 JULY 2021.xlsx
+++ b/input/Lewis World Species List 26 JULY 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01AE2E27-1FBD-4E0B-87B0-CF098D881B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{01AE2E27-1FBD-4E0B-87B0-CF098D881B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C01092-9888-4EB2-AF4D-73EBE099C0F7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13492,8 +13492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1636" workbookViewId="0">
-      <selection activeCell="D1589" sqref="D1589"/>
+    <sheetView tabSelected="1" topLeftCell="A3053" workbookViewId="0">
+      <selection activeCell="D3245" sqref="D3245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -90663,8 +90663,9 @@
       <sortCondition ref="D2:D3480"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D3462">
-    <sortCondition ref="D2:D3462"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H3482">
+    <sortCondition ref="C2:C3482"/>
+    <sortCondition ref="D2:D3482"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>